<commit_message>
UI rejection note script updated
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-RejectionNote.xlsx
+++ b/tests/artifact/script/UI-RejectionNote.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="980">
   <si>
     <t>target</t>
   </si>
@@ -2439,12 +2439,6 @@
     <t>${transport.DateofSupply}</t>
   </si>
   <si>
-    <t>Then user can select the reverse charges</t>
-  </si>
-  <si>
-    <t>${transport.ReverseCharge}</t>
-  </si>
-  <si>
     <t>${invoice.Createitem}</t>
   </si>
   <si>
@@ -2926,6 +2920,9 @@
   </si>
   <si>
     <t>${Total_OrderVal_Val}</t>
+  </si>
+  <si>
+    <t>[NUMBER(${sale.price}) =&gt; multiply(3)]</t>
   </si>
   <si>
     <t>Verify Narration_Header</t>
@@ -10544,12 +10541,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O156"/>
+  <dimension ref="A1:O155"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -11188,76 +11185,78 @@
       <c r="N23" s="71"/>
       <c r="O23" s="62"/>
     </row>
-    <row r="24" ht="23" customHeight="1" spans="1:15">
+    <row r="24" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="26"/>
       <c r="B24" s="30" t="s">
+        <v>766</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>576</v>
+      </c>
+      <c r="E24" s="32" t="s">
         <v>791</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="E24" s="32" t="s">
+      <c r="F24" s="33">
+        <v>2000</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="23"/>
+    </row>
+    <row r="25" s="55" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21" t="s">
         <v>792</v>
       </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="71"/>
-      <c r="O24" s="62"/>
-    </row>
-    <row r="25" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A25" s="26"/>
-      <c r="B25" s="30" t="s">
-        <v>766</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>576</v>
-      </c>
-      <c r="E25" s="32" t="s">
+      <c r="C25" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="E25" s="28" t="s">
         <v>793</v>
       </c>
-      <c r="F25" s="33">
-        <v>2000</v>
-      </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="23"/>
+      <c r="F25" s="28" t="s">
+        <v>794</v>
+      </c>
+      <c r="G25" s="41"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="9"/>
     </row>
     <row r="26" s="55" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A26" s="20"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="21" t="s">
-        <v>794</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>471</v>
-      </c>
-      <c r="E26" s="28" t="s">
         <v>795</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="C26" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>706</v>
+      </c>
+      <c r="E26" s="32" t="s">
         <v>796</v>
       </c>
-      <c r="G26" s="41"/>
+      <c r="F26" s="32" t="s">
+        <v>797</v>
+      </c>
+      <c r="G26" s="32"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="8"/>
@@ -11270,7 +11269,7 @@
     <row r="27" s="55" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A27" s="26"/>
       <c r="B27" s="21" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C27" s="31" t="s">
         <v>30</v>
@@ -11279,10 +11278,10 @@
         <v>706</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G27" s="32"/>
       <c r="H27" s="7"/>
@@ -11294,10 +11293,10 @@
       <c r="N27" s="10"/>
       <c r="O27" s="9"/>
     </row>
-    <row r="28" s="55" customFormat="1" ht="19" customHeight="1" spans="1:15">
+    <row r="28" s="55" customFormat="1" ht="21" customHeight="1" spans="1:15">
       <c r="A28" s="26"/>
       <c r="B28" s="21" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C28" s="31" t="s">
         <v>30</v>
@@ -11306,10 +11305,10 @@
         <v>706</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="G28" s="32"/>
       <c r="H28" s="7"/>
@@ -11324,7 +11323,7 @@
     <row r="29" s="55" customFormat="1" ht="21" customHeight="1" spans="1:15">
       <c r="A29" s="26"/>
       <c r="B29" s="21" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>30</v>
@@ -11333,10 +11332,10 @@
         <v>706</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="G29" s="32"/>
       <c r="H29" s="7"/>
@@ -11351,7 +11350,7 @@
     <row r="30" s="55" customFormat="1" ht="21" customHeight="1" spans="1:15">
       <c r="A30" s="26"/>
       <c r="B30" s="21" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C30" s="31" t="s">
         <v>30</v>
@@ -11360,10 +11359,10 @@
         <v>706</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="G30" s="32"/>
       <c r="H30" s="7"/>
@@ -11378,7 +11377,7 @@
     <row r="31" s="55" customFormat="1" ht="21" customHeight="1" spans="1:15">
       <c r="A31" s="26"/>
       <c r="B31" s="21" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C31" s="31" t="s">
         <v>30</v>
@@ -11387,10 +11386,10 @@
         <v>706</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="G31" s="32"/>
       <c r="H31" s="7"/>
@@ -11402,22 +11401,22 @@
       <c r="N31" s="10"/>
       <c r="O31" s="9"/>
     </row>
-    <row r="32" s="55" customFormat="1" ht="21" customHeight="1" spans="1:15">
+    <row r="32" s="55" customFormat="1" ht="22" customHeight="1" spans="1:15">
       <c r="A32" s="26"/>
       <c r="B32" s="21" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>706</v>
+        <v>576</v>
       </c>
       <c r="E32" s="32" t="s">
-        <v>813</v>
-      </c>
-      <c r="F32" s="32" t="s">
         <v>814</v>
+      </c>
+      <c r="F32" s="33">
+        <v>2000</v>
       </c>
       <c r="G32" s="32"/>
       <c r="H32" s="7"/>
@@ -11429,9 +11428,9 @@
       <c r="N32" s="10"/>
       <c r="O32" s="9"/>
     </row>
-    <row r="33" s="55" customFormat="1" ht="22" customHeight="1" spans="1:15">
+    <row r="33" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A33" s="26"/>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="30" t="s">
         <v>815</v>
       </c>
       <c r="C33" s="31" t="s">
@@ -11447,32 +11446,30 @@
         <v>2000</v>
       </c>
       <c r="G33" s="32"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="9"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="62"/>
     </row>
     <row r="34" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A34" s="26"/>
       <c r="B34" s="30" t="s">
-        <v>817</v>
+        <v>762</v>
       </c>
       <c r="C34" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>576</v>
+        <v>714</v>
       </c>
       <c r="E34" s="32" t="s">
-        <v>818</v>
-      </c>
-      <c r="F34" s="33">
-        <v>2000</v>
-      </c>
+        <v>763</v>
+      </c>
+      <c r="F34" s="33"/>
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
       <c r="I34" s="32"/>
@@ -11486,16 +11483,16 @@
     <row r="35" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A35" s="26"/>
       <c r="B35" s="30" t="s">
-        <v>762</v>
+        <v>817</v>
       </c>
       <c r="C35" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>714</v>
+        <v>253</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>763</v>
+        <v>818</v>
       </c>
       <c r="F35" s="33"/>
       <c r="G35" s="32"/>
@@ -11508,7 +11505,7 @@
       <c r="N35" s="71"/>
       <c r="O35" s="62"/>
     </row>
-    <row r="36" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="36" ht="23" customHeight="1" spans="1:15">
       <c r="A36" s="26"/>
       <c r="B36" s="30" t="s">
         <v>819</v>
@@ -11517,12 +11514,14 @@
         <v>30</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>253</v>
+        <v>576</v>
       </c>
       <c r="E36" s="32" t="s">
         <v>820</v>
       </c>
-      <c r="F36" s="33"/>
+      <c r="F36" s="32" t="s">
+        <v>821</v>
+      </c>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="32"/>
@@ -11533,23 +11532,21 @@
       <c r="N36" s="71"/>
       <c r="O36" s="62"/>
     </row>
-    <row r="37" ht="23" customHeight="1" spans="1:15">
+    <row r="37" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A37" s="26"/>
       <c r="B37" s="30" t="s">
-        <v>821</v>
+        <v>762</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>576</v>
-      </c>
-      <c r="E37" s="32" t="s">
-        <v>822</v>
-      </c>
-      <c r="F37" s="32" t="s">
-        <v>823</v>
-      </c>
+        <v>714</v>
+      </c>
+      <c r="E37" s="39" t="s">
+        <v>763</v>
+      </c>
+      <c r="F37" s="32"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
       <c r="I37" s="32"/>
@@ -11560,21 +11557,23 @@
       <c r="N37" s="71"/>
       <c r="O37" s="62"/>
     </row>
-    <row r="38" customFormat="1" ht="24" customHeight="1" spans="1:15">
+    <row r="38" ht="23" customHeight="1" spans="1:15">
       <c r="A38" s="26"/>
       <c r="B38" s="30" t="s">
-        <v>762</v>
+        <v>815</v>
       </c>
       <c r="C38" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>714</v>
-      </c>
-      <c r="E38" s="39" t="s">
-        <v>763</v>
-      </c>
-      <c r="F38" s="32"/>
+        <v>576</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>816</v>
+      </c>
+      <c r="F38" s="33">
+        <v>2000</v>
+      </c>
       <c r="G38" s="32"/>
       <c r="H38" s="32"/>
       <c r="I38" s="32"/>
@@ -11585,7 +11584,7 @@
       <c r="N38" s="71"/>
       <c r="O38" s="62"/>
     </row>
-    <row r="39" ht="23" customHeight="1" spans="1:15">
+    <row r="39" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A39" s="26"/>
       <c r="B39" s="30" t="s">
         <v>817</v>
@@ -11594,14 +11593,12 @@
         <v>30</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>576</v>
+        <v>253</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>818</v>
-      </c>
-      <c r="F39" s="33">
-        <v>2000</v>
-      </c>
+        <v>822</v>
+      </c>
+      <c r="F39" s="33"/>
       <c r="G39" s="32"/>
       <c r="H39" s="32"/>
       <c r="I39" s="32"/>
@@ -11612,21 +11609,21 @@
       <c r="N39" s="71"/>
       <c r="O39" s="62"/>
     </row>
-    <row r="40" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="40" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A40" s="26"/>
       <c r="B40" s="30" t="s">
-        <v>819</v>
+        <v>762</v>
       </c>
       <c r="C40" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>824</v>
-      </c>
-      <c r="F40" s="33"/>
+        <v>714</v>
+      </c>
+      <c r="E40" s="39" t="s">
+        <v>763</v>
+      </c>
+      <c r="F40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="32"/>
@@ -11637,48 +11634,48 @@
       <c r="N40" s="71"/>
       <c r="O40" s="62"/>
     </row>
-    <row r="41" customFormat="1" ht="24" customHeight="1" spans="1:15">
-      <c r="A41" s="26"/>
-      <c r="B41" s="30" t="s">
-        <v>762</v>
-      </c>
-      <c r="C41" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="32" t="s">
-        <v>714</v>
-      </c>
-      <c r="E41" s="39" t="s">
-        <v>763</v>
-      </c>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="73"/>
-      <c r="K41" s="62"/>
-      <c r="L41" s="71"/>
-      <c r="M41" s="72"/>
-      <c r="N41" s="71"/>
-      <c r="O41" s="62"/>
+    <row r="41" s="55" customFormat="1" spans="1:15">
+      <c r="A41" s="1"/>
+      <c r="B41" s="21" t="s">
+        <v>823</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="E41" s="55" t="s">
+        <v>824</v>
+      </c>
+      <c r="F41" s="28" t="s">
+        <v>825</v>
+      </c>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="70"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="23"/>
     </row>
     <row r="42" s="55" customFormat="1" spans="1:15">
       <c r="A42" s="1"/>
       <c r="B42" s="21" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>493</v>
+        <v>536</v>
       </c>
       <c r="E42" s="55" t="s">
-        <v>826</v>
-      </c>
-      <c r="F42" s="28" t="s">
         <v>827</v>
       </c>
+      <c r="F42" s="28"/>
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="28"/>
@@ -11689,21 +11686,22 @@
       <c r="N42" s="24"/>
       <c r="O42" s="23"/>
     </row>
-    <row r="43" s="55" customFormat="1" spans="1:15">
-      <c r="A43" s="1"/>
+    <row r="43" s="1" customFormat="1" spans="2:15">
       <c r="B43" s="21" t="s">
         <v>828</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="28" t="s">
-        <v>536</v>
-      </c>
-      <c r="E43" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>576</v>
+      </c>
+      <c r="E43" s="28" t="s">
         <v>829</v>
       </c>
-      <c r="F43" s="28"/>
+      <c r="F43" s="33">
+        <v>2000</v>
+      </c>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
@@ -11714,21 +11712,24 @@
       <c r="N43" s="24"/>
       <c r="O43" s="23"/>
     </row>
-    <row r="44" s="1" customFormat="1" spans="2:15">
+    <row r="44" s="42" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="A44" s="26" t="s">
+        <v>830</v>
+      </c>
       <c r="B44" s="21" t="s">
-        <v>830</v>
+        <v>757</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="32" t="s">
+      <c r="D44" s="28" t="s">
         <v>576</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>831</v>
-      </c>
-      <c r="F44" s="33">
-        <v>2000</v>
+        <v>758</v>
+      </c>
+      <c r="F44" s="29">
+        <v>4000</v>
       </c>
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
@@ -11740,12 +11741,9 @@
       <c r="N44" s="24"/>
       <c r="O44" s="23"/>
     </row>
-    <row r="45" s="42" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A45" s="26" t="s">
-        <v>832</v>
-      </c>
+    <row r="45" s="42" customFormat="1" ht="29" customHeight="1" spans="2:15">
       <c r="B45" s="21" t="s">
-        <v>757</v>
+        <v>831</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>30</v>
@@ -11754,10 +11752,10 @@
         <v>576</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>758</v>
+        <v>832</v>
       </c>
       <c r="F45" s="29">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="G45" s="28"/>
       <c r="H45" s="28"/>
@@ -11769,22 +11767,21 @@
       <c r="N45" s="24"/>
       <c r="O45" s="23"/>
     </row>
-    <row r="46" s="42" customFormat="1" ht="29" customHeight="1" spans="2:15">
-      <c r="B46" s="21" t="s">
-        <v>833</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="28" t="s">
-        <v>576</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>834</v>
-      </c>
-      <c r="F46" s="29">
-        <v>2000</v>
-      </c>
+    <row r="46" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A46" s="26"/>
+      <c r="B46" s="30" t="s">
+        <v>762</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>768</v>
+      </c>
+      <c r="F46" s="33"/>
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
       <c r="I46" s="28"/>
@@ -11795,21 +11792,23 @@
       <c r="N46" s="24"/>
       <c r="O46" s="23"/>
     </row>
-    <row r="47" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="47" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A47" s="26"/>
       <c r="B47" s="30" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="C47" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>714</v>
+        <v>576</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>768</v>
-      </c>
-      <c r="F47" s="33"/>
+        <v>833</v>
+      </c>
+      <c r="F47" s="33">
+        <v>2000</v>
+      </c>
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
       <c r="I47" s="28"/>
@@ -11820,23 +11819,21 @@
       <c r="N47" s="24"/>
       <c r="O47" s="23"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="48" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A48" s="26"/>
       <c r="B48" s="30" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="C48" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>576</v>
+        <v>714</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>835</v>
-      </c>
-      <c r="F48" s="33">
-        <v>2000</v>
-      </c>
+        <v>768</v>
+      </c>
+      <c r="F48" s="33"/>
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
@@ -11847,128 +11844,128 @@
       <c r="N48" s="24"/>
       <c r="O48" s="23"/>
     </row>
-    <row r="49" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A49" s="26"/>
+    <row r="49" customFormat="1" ht="45" customHeight="1" spans="2:15">
       <c r="B49" s="30" t="s">
-        <v>762</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" s="32" t="s">
-        <v>714</v>
-      </c>
-      <c r="E49" s="32" t="s">
-        <v>768</v>
-      </c>
-      <c r="F49" s="33"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="70"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="24"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="24"/>
-      <c r="O49" s="23"/>
-    </row>
-    <row r="50" customFormat="1" ht="45" customHeight="1" spans="2:15">
-      <c r="B50" s="30" t="s">
+        <v>834</v>
+      </c>
+      <c r="C49" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>576</v>
+      </c>
+      <c r="E49" s="37" t="s">
+        <v>835</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>763</v>
+      </c>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="73"/>
+      <c r="K49" s="62"/>
+      <c r="L49" s="71"/>
+      <c r="M49" s="72"/>
+      <c r="N49" s="71"/>
+      <c r="O49" s="62"/>
+    </row>
+    <row r="50" s="81" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A50" s="43"/>
+      <c r="B50" s="44" t="s">
+        <v>771</v>
+      </c>
+      <c r="C50" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>692</v>
+      </c>
+      <c r="E50" s="46" t="s">
         <v>836</v>
       </c>
-      <c r="C50" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" s="37" t="s">
-        <v>576</v>
-      </c>
-      <c r="E50" s="37" t="s">
+      <c r="F50" s="82" t="s">
         <v>837</v>
       </c>
-      <c r="F50" s="32" t="s">
-        <v>763</v>
-      </c>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="73"/>
-      <c r="K50" s="62"/>
-      <c r="L50" s="71"/>
-      <c r="M50" s="72"/>
-      <c r="N50" s="71"/>
-      <c r="O50" s="62"/>
-    </row>
-    <row r="51" s="81" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A51" s="43"/>
-      <c r="B51" s="44" t="s">
-        <v>771</v>
-      </c>
-      <c r="C51" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="46" t="s">
-        <v>692</v>
-      </c>
-      <c r="E51" s="46" t="s">
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="83"/>
+      <c r="L50" s="84"/>
+      <c r="M50" s="85"/>
+      <c r="N50" s="84"/>
+      <c r="O50" s="83"/>
+    </row>
+    <row r="51" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A51" s="48"/>
+      <c r="B51" s="49" t="s">
         <v>838</v>
       </c>
-      <c r="F51" s="82" t="s">
+      <c r="C51" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="51" t="s">
+        <v>530</v>
+      </c>
+      <c r="E51" s="52" t="s">
         <v>839</v>
       </c>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="83"/>
-      <c r="L51" s="84"/>
-      <c r="M51" s="85"/>
-      <c r="N51" s="84"/>
-      <c r="O51" s="83"/>
-    </row>
-    <row r="52" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A52" s="48"/>
-      <c r="B52" s="49" t="s">
+      <c r="F51" s="53" t="s">
+        <v>797</v>
+      </c>
+      <c r="G51" s="54"/>
+      <c r="H51" s="54"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="75"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="77"/>
+      <c r="M51" s="78"/>
+      <c r="N51" s="77"/>
+      <c r="O51" s="76"/>
+    </row>
+    <row r="52" ht="23" customHeight="1" spans="1:15">
+      <c r="A52" s="26"/>
+      <c r="B52" s="30" t="s">
         <v>840</v>
       </c>
-      <c r="C52" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="D52" s="51" t="s">
-        <v>253</v>
-      </c>
-      <c r="E52" s="52" t="s">
+      <c r="C52" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>706</v>
+      </c>
+      <c r="E52" s="32" t="s">
         <v>841</v>
       </c>
-      <c r="F52" s="53" t="s">
-        <v>799</v>
-      </c>
-      <c r="G52" s="54"/>
-      <c r="H52" s="54"/>
-      <c r="I52" s="54"/>
-      <c r="J52" s="75"/>
-      <c r="K52" s="76"/>
-      <c r="L52" s="77"/>
-      <c r="M52" s="78"/>
-      <c r="N52" s="77"/>
-      <c r="O52" s="76"/>
+      <c r="F52" s="32" t="s">
+        <v>842</v>
+      </c>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="73"/>
+      <c r="K52" s="62"/>
+      <c r="L52" s="71"/>
+      <c r="M52" s="72"/>
+      <c r="N52" s="71"/>
+      <c r="O52" s="62"/>
     </row>
     <row r="53" ht="23" customHeight="1" spans="1:15">
       <c r="A53" s="26"/>
       <c r="B53" s="30" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C53" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>706</v>
+        <v>363</v>
       </c>
       <c r="E53" s="32" t="s">
-        <v>843</v>
-      </c>
-      <c r="F53" s="32" t="s">
         <v>844</v>
       </c>
+      <c r="F53" s="32"/>
       <c r="G53" s="32"/>
       <c r="H53" s="32"/>
       <c r="I53" s="32"/>
@@ -11982,18 +11979,20 @@
     <row r="54" ht="23" customHeight="1" spans="1:15">
       <c r="A54" s="26"/>
       <c r="B54" s="30" t="s">
-        <v>845</v>
+        <v>815</v>
       </c>
       <c r="C54" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>363</v>
+        <v>576</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>846</v>
-      </c>
-      <c r="F54" s="32"/>
+        <v>816</v>
+      </c>
+      <c r="F54" s="33">
+        <v>2000</v>
+      </c>
       <c r="G54" s="32"/>
       <c r="H54" s="32"/>
       <c r="I54" s="32"/>
@@ -12004,48 +12003,48 @@
       <c r="N54" s="71"/>
       <c r="O54" s="62"/>
     </row>
-    <row r="55" ht="23" customHeight="1" spans="1:15">
+    <row r="55" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A55" s="26"/>
       <c r="B55" s="30" t="s">
-        <v>817</v>
+        <v>762</v>
       </c>
       <c r="C55" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>576</v>
+        <v>714</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>818</v>
-      </c>
-      <c r="F55" s="33">
-        <v>2000</v>
-      </c>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="73"/>
-      <c r="K55" s="62"/>
-      <c r="L55" s="71"/>
-      <c r="M55" s="72"/>
-      <c r="N55" s="71"/>
-      <c r="O55" s="62"/>
-    </row>
-    <row r="56" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A56" s="26"/>
-      <c r="B56" s="30" t="s">
-        <v>762</v>
-      </c>
-      <c r="C56" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="32" t="s">
-        <v>714</v>
-      </c>
-      <c r="E56" s="32" t="s">
         <v>768</v>
       </c>
-      <c r="F56" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="70"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="24"/>
+      <c r="M55" s="22"/>
+      <c r="N55" s="24"/>
+      <c r="O55" s="23"/>
+    </row>
+    <row r="56" s="55" customFormat="1" spans="1:15">
+      <c r="A56" s="1"/>
+      <c r="B56" s="21" t="s">
+        <v>845</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="E56" s="55" t="s">
+        <v>846</v>
+      </c>
+      <c r="F56" s="28" t="s">
+        <v>847</v>
+      </c>
       <c r="G56" s="28"/>
       <c r="H56" s="28"/>
       <c r="I56" s="28"/>
@@ -12056,24 +12055,21 @@
       <c r="N56" s="24"/>
       <c r="O56" s="23"/>
     </row>
-    <row r="57" s="55" customFormat="1" spans="1:15">
-      <c r="A57" s="1"/>
-      <c r="B57" s="21" t="s">
-        <v>847</v>
+    <row r="57" s="55" customFormat="1" ht="15.5" spans="1:15">
+      <c r="A57" s="26"/>
+      <c r="B57" s="56" t="s">
+        <v>848</v>
       </c>
       <c r="C57" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>493</v>
-      </c>
-      <c r="E57" s="55" t="s">
-        <v>848</v>
-      </c>
-      <c r="F57" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="E57" s="28" t="s">
         <v>849</v>
       </c>
-      <c r="G57" s="28"/>
+      <c r="G57" s="57"/>
       <c r="H57" s="28"/>
       <c r="I57" s="28"/>
       <c r="J57" s="70"/>
@@ -12083,21 +12079,23 @@
       <c r="N57" s="24"/>
       <c r="O57" s="23"/>
     </row>
-    <row r="58" s="55" customFormat="1" ht="15.5" spans="1:15">
-      <c r="A58" s="26"/>
-      <c r="B58" s="56" t="s">
-        <v>850</v>
+    <row r="58" s="1" customFormat="1" spans="2:15">
+      <c r="B58" s="21" t="s">
+        <v>828</v>
       </c>
       <c r="C58" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D58" s="28" t="s">
-        <v>253</v>
+      <c r="D58" s="32" t="s">
+        <v>576</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>851</v>
-      </c>
-      <c r="G58" s="57"/>
+        <v>829</v>
+      </c>
+      <c r="F58" s="33">
+        <v>2000</v>
+      </c>
+      <c r="G58" s="28"/>
       <c r="H58" s="28"/>
       <c r="I58" s="28"/>
       <c r="J58" s="70"/>
@@ -12107,74 +12105,68 @@
       <c r="N58" s="24"/>
       <c r="O58" s="23"/>
     </row>
-    <row r="59" s="1" customFormat="1" spans="2:15">
-      <c r="B59" s="21" t="s">
-        <v>830</v>
-      </c>
-      <c r="C59" s="27" t="s">
+    <row r="59" s="58" customFormat="1" ht="28" spans="1:15">
+      <c r="A59" s="20" t="s">
+        <v>850</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="C59" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D59" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="E59" s="33" t="s">
+        <v>852</v>
+      </c>
+      <c r="G59" s="33"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="73"/>
+      <c r="K59" s="62"/>
+      <c r="L59" s="71"/>
+      <c r="M59" s="72"/>
+      <c r="N59" s="71"/>
+      <c r="O59" s="62"/>
+    </row>
+    <row r="60" customFormat="1" ht="15.5" spans="2:10">
+      <c r="B60" s="21" t="s">
+        <v>853</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="28" t="s">
         <v>576</v>
       </c>
-      <c r="E59" s="28" t="s">
-        <v>831</v>
-      </c>
-      <c r="F59" s="33">
-        <v>2000</v>
-      </c>
-      <c r="G59" s="28"/>
-      <c r="H59" s="28"/>
-      <c r="I59" s="28"/>
-      <c r="J59" s="70"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="24"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="24"/>
-      <c r="O59" s="23"/>
-    </row>
-    <row r="60" s="58" customFormat="1" ht="28" spans="1:15">
-      <c r="A60" s="20" t="s">
-        <v>852</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>853</v>
-      </c>
-      <c r="C60" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D60" s="32" t="s">
+      <c r="E60" s="32" t="s">
+        <v>854</v>
+      </c>
+      <c r="F60" s="37" t="s">
+        <v>855</v>
+      </c>
+      <c r="G60" s="32"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="70"/>
+    </row>
+    <row r="61" customFormat="1" ht="15.5" spans="1:10">
+      <c r="A61" s="20"/>
+      <c r="B61" s="21" t="s">
+        <v>856</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="E60" s="33" t="s">
-        <v>854</v>
-      </c>
-      <c r="G60" s="33"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-      <c r="J60" s="73"/>
-      <c r="K60" s="62"/>
-      <c r="L60" s="71"/>
-      <c r="M60" s="72"/>
-      <c r="N60" s="71"/>
-      <c r="O60" s="62"/>
-    </row>
-    <row r="61" customFormat="1" ht="15.5" spans="2:10">
-      <c r="B61" s="21" t="s">
-        <v>855</v>
-      </c>
-      <c r="C61" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D61" s="28" t="s">
-        <v>576</v>
-      </c>
-      <c r="E61" s="32" t="s">
-        <v>856</v>
-      </c>
-      <c r="F61" s="37" t="s">
+      <c r="E61" s="28" t="s">
         <v>857</v>
       </c>
+      <c r="F61" s="28"/>
       <c r="G61" s="32"/>
       <c r="H61" s="28"/>
       <c r="I61" s="28"/>
@@ -12182,19 +12174,19 @@
     </row>
     <row r="62" customFormat="1" ht="15.5" spans="1:10">
       <c r="A62" s="20"/>
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="59" t="s">
         <v>858</v>
       </c>
-      <c r="C62" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D62" s="28" t="s">
+      <c r="C62" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="37" t="s">
         <v>363</v>
       </c>
       <c r="E62" s="28" t="s">
         <v>859</v>
       </c>
-      <c r="F62" s="28"/>
+      <c r="F62" s="60"/>
       <c r="G62" s="32"/>
       <c r="H62" s="28"/>
       <c r="I62" s="28"/>
@@ -12202,19 +12194,19 @@
     </row>
     <row r="63" customFormat="1" ht="15.5" spans="1:10">
       <c r="A63" s="20"/>
-      <c r="B63" s="59" t="s">
+      <c r="B63" s="21" t="s">
         <v>860</v>
       </c>
-      <c r="C63" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D63" s="37" t="s">
-        <v>363</v>
+      <c r="C63" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>714</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>861</v>
-      </c>
-      <c r="F63" s="60"/>
+        <v>855</v>
+      </c>
+      <c r="F63" s="40"/>
       <c r="G63" s="32"/>
       <c r="H63" s="28"/>
       <c r="I63" s="28"/>
@@ -12222,19 +12214,19 @@
     </row>
     <row r="64" customFormat="1" ht="15.5" spans="1:10">
       <c r="A64" s="20"/>
-      <c r="B64" s="21" t="s">
-        <v>862</v>
-      </c>
-      <c r="C64" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D64" s="28" t="s">
-        <v>714</v>
+      <c r="B64" s="59" t="s">
+        <v>861</v>
+      </c>
+      <c r="C64" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" s="37" t="s">
+        <v>363</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>857</v>
-      </c>
-      <c r="F64" s="40"/>
+        <v>859</v>
+      </c>
+      <c r="F64" s="60"/>
       <c r="G64" s="32"/>
       <c r="H64" s="28"/>
       <c r="I64" s="28"/>
@@ -12242,17 +12234,17 @@
     </row>
     <row r="65" customFormat="1" ht="15.5" spans="1:10">
       <c r="A65" s="20"/>
-      <c r="B65" s="59" t="s">
-        <v>863</v>
-      </c>
-      <c r="C65" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D65" s="37" t="s">
-        <v>363</v>
+      <c r="B65" s="21" t="s">
+        <v>860</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>714</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="F65" s="60"/>
       <c r="G65" s="32"/>
@@ -12262,17 +12254,17 @@
     </row>
     <row r="66" customFormat="1" ht="15.5" spans="1:10">
       <c r="A66" s="20"/>
-      <c r="B66" s="21" t="s">
+      <c r="B66" s="59" t="s">
         <v>862</v>
       </c>
-      <c r="C66" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="28" t="s">
-        <v>714</v>
+      <c r="C66" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="37" t="s">
+        <v>363</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>857</v>
+        <v>863</v>
       </c>
       <c r="F66" s="60"/>
       <c r="G66" s="32"/>
@@ -12280,57 +12272,59 @@
       <c r="I66" s="28"/>
       <c r="J66" s="70"/>
     </row>
-    <row r="67" customFormat="1" ht="15.5" spans="1:10">
-      <c r="A67" s="20"/>
-      <c r="B67" s="59" t="s">
+    <row r="67" customFormat="1" ht="45" customHeight="1" spans="1:15">
+      <c r="A67" s="26"/>
+      <c r="B67" s="30" t="s">
         <v>864</v>
       </c>
       <c r="C67" s="36" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>363</v>
-      </c>
-      <c r="E67" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="E67" t="s">
         <v>865</v>
       </c>
-      <c r="F67" s="60"/>
+      <c r="F67" s="55" t="s">
+        <v>866</v>
+      </c>
       <c r="G67" s="32"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="70"/>
-    </row>
-    <row r="68" customFormat="1" ht="45" customHeight="1" spans="1:15">
-      <c r="A68" s="26"/>
-      <c r="B68" s="30" t="s">
-        <v>866</v>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="73"/>
+      <c r="K67" s="62"/>
+      <c r="L67" s="71"/>
+      <c r="M67" s="72"/>
+      <c r="N67" s="71"/>
+      <c r="O67" s="62"/>
+    </row>
+    <row r="68" customFormat="1" ht="15.5" spans="1:10">
+      <c r="A68" s="20"/>
+      <c r="B68" s="59" t="s">
+        <v>867</v>
       </c>
       <c r="C68" s="36" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>471</v>
-      </c>
-      <c r="E68" t="s">
-        <v>867</v>
-      </c>
-      <c r="F68" s="55" t="s">
+        <v>706</v>
+      </c>
+      <c r="E68" s="28" t="s">
         <v>868</v>
       </c>
+      <c r="F68" s="60" t="s">
+        <v>869</v>
+      </c>
       <c r="G68" s="32"/>
-      <c r="H68" s="32"/>
-      <c r="I68" s="32"/>
-      <c r="J68" s="73"/>
-      <c r="K68" s="62"/>
-      <c r="L68" s="71"/>
-      <c r="M68" s="72"/>
-      <c r="N68" s="71"/>
-      <c r="O68" s="62"/>
+      <c r="H68" s="28"/>
+      <c r="I68" s="28"/>
+      <c r="J68" s="70"/>
     </row>
     <row r="69" customFormat="1" ht="15.5" spans="1:10">
       <c r="A69" s="20"/>
       <c r="B69" s="59" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C69" s="36" t="s">
         <v>30</v>
@@ -12339,10 +12333,10 @@
         <v>706</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="F69" s="60" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="G69" s="32"/>
       <c r="H69" s="28"/>
@@ -12351,142 +12345,145 @@
     </row>
     <row r="70" customFormat="1" ht="15.5" spans="1:10">
       <c r="A70" s="20"/>
-      <c r="B70" s="59" t="s">
+      <c r="B70" s="21" t="s">
         <v>872</v>
       </c>
-      <c r="C70" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D70" s="37" t="s">
-        <v>706</v>
-      </c>
-      <c r="E70" s="28" t="s">
+      <c r="C70" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="E70" s="70" t="s">
         <v>873</v>
       </c>
-      <c r="F70" s="60" t="s">
-        <v>871</v>
-      </c>
-      <c r="G70" s="32"/>
-      <c r="H70" s="28"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="70"/>
+      <c r="F70" s="79" t="s">
+        <v>752</v>
+      </c>
+      <c r="G70" s="55" t="s">
+        <v>874</v>
+      </c>
+      <c r="H70" s="58" t="s">
+        <v>875</v>
+      </c>
+      <c r="I70" s="58"/>
+      <c r="J70" s="58"/>
     </row>
     <row r="71" customFormat="1" ht="15.5" spans="1:10">
       <c r="A71" s="20"/>
       <c r="B71" s="21" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="C71" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="28" t="s">
-        <v>486</v>
+        <v>30</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>363</v>
       </c>
       <c r="E71" s="70" t="s">
-        <v>875</v>
-      </c>
-      <c r="F71" s="79" t="s">
-        <v>752</v>
-      </c>
-      <c r="G71" s="55" t="s">
-        <v>876</v>
-      </c>
-      <c r="H71" s="58" t="s">
         <v>877</v>
       </c>
-      <c r="I71" s="58"/>
-      <c r="J71" s="58"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="70"/>
     </row>
     <row r="72" customFormat="1" ht="15.5" spans="1:10">
       <c r="A72" s="20"/>
       <c r="B72" s="21" t="s">
-        <v>878</v>
+        <v>860</v>
       </c>
       <c r="C72" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D72" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="E72" s="70" t="s">
-        <v>879</v>
-      </c>
-      <c r="F72" s="33"/>
+      <c r="D72" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="E72" s="28" t="s">
+        <v>855</v>
+      </c>
+      <c r="F72" s="60"/>
       <c r="G72" s="32"/>
       <c r="H72" s="28"/>
       <c r="I72" s="28"/>
       <c r="J72" s="70"/>
     </row>
     <row r="73" customFormat="1" ht="15.5" spans="1:10">
-      <c r="A73" s="20"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="21" t="s">
-        <v>862</v>
+        <v>872</v>
       </c>
       <c r="C73" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>714</v>
-      </c>
-      <c r="E73" s="28" t="s">
-        <v>857</v>
-      </c>
-      <c r="F73" s="60"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="70"/>
+        <v>650</v>
+      </c>
+      <c r="E73" t="s">
+        <v>878</v>
+      </c>
+      <c r="F73" s="32" t="s">
+        <v>879</v>
+      </c>
+      <c r="G73" s="55" t="s">
+        <v>880</v>
+      </c>
+      <c r="H73" s="58"/>
+      <c r="I73" s="32"/>
+      <c r="J73" s="73"/>
     </row>
     <row r="74" customFormat="1" ht="15.5" spans="1:10">
-      <c r="A74" s="26"/>
+      <c r="A74" s="20"/>
       <c r="B74" s="21" t="s">
-        <v>874</v>
+        <v>881</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>650</v>
-      </c>
-      <c r="E74" t="s">
-        <v>880</v>
-      </c>
-      <c r="F74" s="32" t="s">
-        <v>881</v>
-      </c>
-      <c r="G74" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="E74" s="70" t="s">
         <v>882</v>
       </c>
+      <c r="F74" t="s">
+        <v>883</v>
+      </c>
+      <c r="G74" s="32"/>
       <c r="H74" s="58"/>
-      <c r="I74" s="32"/>
-      <c r="J74" s="73"/>
-    </row>
-    <row r="75" customFormat="1" ht="15.5" spans="1:10">
-      <c r="A75" s="20"/>
-      <c r="B75" s="21" t="s">
-        <v>883</v>
-      </c>
-      <c r="C75" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D75" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E75" s="70" t="s">
+      <c r="I74" s="58"/>
+      <c r="J74" s="58"/>
+    </row>
+    <row r="75" s="55" customFormat="1" ht="42" spans="1:15">
+      <c r="A75" s="26" t="s">
         <v>884</v>
       </c>
-      <c r="F75" t="s">
+      <c r="B75" s="30" t="s">
         <v>885</v>
       </c>
+      <c r="C75" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="E75" s="32" t="s">
+        <v>886</v>
+      </c>
+      <c r="F75" s="32"/>
       <c r="G75" s="32"/>
-      <c r="H75" s="58"/>
-      <c r="I75" s="58"/>
-      <c r="J75" s="58"/>
-    </row>
-    <row r="76" s="55" customFormat="1" ht="42" spans="1:15">
-      <c r="A76" s="26" t="s">
-        <v>886</v>
-      </c>
+      <c r="H75" s="32"/>
+      <c r="I75" s="32"/>
+      <c r="J75" s="73"/>
+      <c r="K75" s="62"/>
+      <c r="L75" s="71"/>
+      <c r="M75" s="72"/>
+      <c r="N75" s="71"/>
+      <c r="O75" s="62"/>
+    </row>
+    <row r="76" customFormat="1" ht="15.5" spans="1:15">
+      <c r="A76" s="26"/>
       <c r="B76" s="30" t="s">
         <v>887</v>
       </c>
@@ -12494,12 +12491,14 @@
         <v>30</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>253</v>
+        <v>319</v>
       </c>
       <c r="E76" s="32" t="s">
         <v>888</v>
       </c>
-      <c r="F76" s="32"/>
+      <c r="F76" s="32" t="s">
+        <v>775</v>
+      </c>
       <c r="G76" s="32"/>
       <c r="H76" s="32"/>
       <c r="I76" s="32"/>
@@ -12524,8 +12523,8 @@
       <c r="E77" s="32" t="s">
         <v>890</v>
       </c>
-      <c r="F77" s="32" t="s">
-        <v>775</v>
+      <c r="F77" s="7" t="s">
+        <v>782</v>
       </c>
       <c r="G77" s="32"/>
       <c r="H77" s="32"/>
@@ -12552,7 +12551,7 @@
         <v>892</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>782</v>
+        <v>893</v>
       </c>
       <c r="G78" s="32"/>
       <c r="H78" s="32"/>
@@ -12567,7 +12566,7 @@
     <row r="79" customFormat="1" ht="15.5" spans="1:15">
       <c r="A79" s="26"/>
       <c r="B79" s="30" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C79" s="31" t="s">
         <v>30</v>
@@ -12576,10 +12575,10 @@
         <v>319</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="G79" s="32"/>
       <c r="H79" s="32"/>
@@ -12594,7 +12593,7 @@
     <row r="80" customFormat="1" ht="15.5" spans="1:15">
       <c r="A80" s="26"/>
       <c r="B80" s="30" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C80" s="31" t="s">
         <v>30</v>
@@ -12603,10 +12602,10 @@
         <v>319</v>
       </c>
       <c r="E80" s="32" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="G80" s="32"/>
       <c r="H80" s="32"/>
@@ -12621,7 +12620,7 @@
     <row r="81" customFormat="1" ht="15.5" spans="1:15">
       <c r="A81" s="26"/>
       <c r="B81" s="30" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C81" s="31" t="s">
         <v>30</v>
@@ -12630,10 +12629,10 @@
         <v>319</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>900</v>
-      </c>
-      <c r="F81" s="7" t="s">
         <v>901</v>
+      </c>
+      <c r="F81" s="29" t="s">
+        <v>902</v>
       </c>
       <c r="G81" s="32"/>
       <c r="H81" s="32"/>
@@ -12648,7 +12647,7 @@
     <row r="82" customFormat="1" ht="15.5" spans="1:15">
       <c r="A82" s="26"/>
       <c r="B82" s="30" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C82" s="31" t="s">
         <v>30</v>
@@ -12657,10 +12656,10 @@
         <v>319</v>
       </c>
       <c r="E82" s="32" t="s">
-        <v>903</v>
-      </c>
-      <c r="F82" s="29" t="s">
         <v>904</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>874</v>
       </c>
       <c r="G82" s="32"/>
       <c r="H82" s="32"/>
@@ -12672,22 +12671,22 @@
       <c r="N82" s="71"/>
       <c r="O82" s="62"/>
     </row>
-    <row r="83" customFormat="1" ht="15.5" spans="1:15">
+    <row r="83" customFormat="1" ht="36" customHeight="1" spans="1:15">
       <c r="A83" s="26"/>
       <c r="B83" s="30" t="s">
         <v>905</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D83" s="32" t="s">
-        <v>319</v>
+        <v>471</v>
       </c>
       <c r="E83" s="32" t="s">
         <v>906</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>876</v>
+        <v>907</v>
       </c>
       <c r="G83" s="32"/>
       <c r="H83" s="32"/>
@@ -12699,22 +12698,22 @@
       <c r="N83" s="71"/>
       <c r="O83" s="62"/>
     </row>
-    <row r="84" customFormat="1" ht="36" customHeight="1" spans="1:15">
+    <row r="84" customFormat="1" ht="15.5" spans="1:15">
       <c r="A84" s="26"/>
       <c r="B84" s="30" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D84" s="32" t="s">
-        <v>471</v>
+        <v>319</v>
       </c>
       <c r="E84" s="32" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="G84" s="32"/>
       <c r="H84" s="32"/>
@@ -12729,7 +12728,7 @@
     <row r="85" customFormat="1" ht="15.5" spans="1:15">
       <c r="A85" s="26"/>
       <c r="B85" s="30" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C85" s="31" t="s">
         <v>30</v>
@@ -12738,10 +12737,10 @@
         <v>319</v>
       </c>
       <c r="E85" s="32" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>912</v>
+        <v>827</v>
       </c>
       <c r="G85" s="32"/>
       <c r="H85" s="32"/>
@@ -12767,8 +12766,8 @@
       <c r="E86" s="32" t="s">
         <v>914</v>
       </c>
-      <c r="F86" s="7" t="s">
-        <v>829</v>
+      <c r="F86" s="29" t="s">
+        <v>915</v>
       </c>
       <c r="G86" s="32"/>
       <c r="H86" s="32"/>
@@ -12783,7 +12782,7 @@
     <row r="87" customFormat="1" ht="15.5" spans="1:15">
       <c r="A87" s="26"/>
       <c r="B87" s="30" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C87" s="31" t="s">
         <v>30</v>
@@ -12792,10 +12791,10 @@
         <v>319</v>
       </c>
       <c r="E87" s="32" t="s">
-        <v>916</v>
-      </c>
-      <c r="F87" s="29" t="s">
         <v>917</v>
+      </c>
+      <c r="F87" s="32" t="s">
+        <v>797</v>
       </c>
       <c r="G87" s="32"/>
       <c r="H87" s="32"/>
@@ -12816,13 +12815,13 @@
         <v>30</v>
       </c>
       <c r="D88" s="32" t="s">
-        <v>319</v>
+        <v>535</v>
       </c>
       <c r="E88" s="32" t="s">
         <v>919</v>
       </c>
       <c r="F88" s="32" t="s">
-        <v>799</v>
+        <v>920</v>
       </c>
       <c r="G88" s="32"/>
       <c r="H88" s="32"/>
@@ -12837,19 +12836,19 @@
     <row r="89" customFormat="1" ht="15.5" spans="1:15">
       <c r="A89" s="26"/>
       <c r="B89" s="30" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C89" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D89" s="32" t="s">
-        <v>535</v>
+        <v>319</v>
       </c>
       <c r="E89" s="32" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F89" s="32" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="G89" s="32"/>
       <c r="H89" s="32"/>
@@ -12861,10 +12860,10 @@
       <c r="N89" s="71"/>
       <c r="O89" s="62"/>
     </row>
-    <row r="90" customFormat="1" ht="15.5" spans="1:15">
+    <row r="90" customFormat="1" ht="16.5" spans="1:15">
       <c r="A90" s="26"/>
       <c r="B90" s="30" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C90" s="31" t="s">
         <v>30</v>
@@ -12873,10 +12872,10 @@
         <v>319</v>
       </c>
       <c r="E90" s="32" t="s">
-        <v>924</v>
-      </c>
-      <c r="F90" s="32" t="s">
         <v>925</v>
+      </c>
+      <c r="F90" s="80" t="s">
+        <v>926</v>
       </c>
       <c r="G90" s="32"/>
       <c r="H90" s="32"/>
@@ -12891,7 +12890,7 @@
     <row r="91" customFormat="1" ht="16.5" spans="1:15">
       <c r="A91" s="26"/>
       <c r="B91" s="30" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C91" s="31" t="s">
         <v>30</v>
@@ -12900,10 +12899,10 @@
         <v>319</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="F91" s="80" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G91" s="32"/>
       <c r="H91" s="32"/>
@@ -12915,7 +12914,7 @@
       <c r="N91" s="71"/>
       <c r="O91" s="62"/>
     </row>
-    <row r="92" customFormat="1" ht="16.5" spans="1:15">
+    <row r="92" customFormat="1" ht="15.5" spans="1:15">
       <c r="A92" s="26"/>
       <c r="B92" s="30" t="s">
         <v>929</v>
@@ -12929,8 +12928,8 @@
       <c r="E92" s="32" t="s">
         <v>930</v>
       </c>
-      <c r="F92" s="80" t="s">
-        <v>928</v>
+      <c r="F92" s="32" t="s">
+        <v>931</v>
       </c>
       <c r="G92" s="32"/>
       <c r="H92" s="32"/>
@@ -12945,7 +12944,7 @@
     <row r="93" customFormat="1" ht="15.5" spans="1:15">
       <c r="A93" s="26"/>
       <c r="B93" s="30" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C93" s="31" t="s">
         <v>30</v>
@@ -12954,10 +12953,10 @@
         <v>319</v>
       </c>
       <c r="E93" s="32" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="F93" s="32" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="G93" s="32"/>
       <c r="H93" s="32"/>
@@ -12972,7 +12971,7 @@
     <row r="94" customFormat="1" ht="15.5" spans="1:15">
       <c r="A94" s="26"/>
       <c r="B94" s="30" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C94" s="31" t="s">
         <v>30</v>
@@ -12981,10 +12980,10 @@
         <v>319</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="F94" s="32" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="G94" s="32"/>
       <c r="H94" s="32"/>
@@ -12999,7 +12998,7 @@
     <row r="95" customFormat="1" ht="15.5" spans="1:15">
       <c r="A95" s="26"/>
       <c r="B95" s="30" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C95" s="31" t="s">
         <v>30</v>
@@ -13008,10 +13007,10 @@
         <v>319</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="F95" s="32" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="G95" s="32"/>
       <c r="H95" s="32"/>
@@ -13026,7 +13025,7 @@
     <row r="96" customFormat="1" ht="15.5" spans="1:15">
       <c r="A96" s="26"/>
       <c r="B96" s="30" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C96" s="31" t="s">
         <v>30</v>
@@ -13035,10 +13034,10 @@
         <v>319</v>
       </c>
       <c r="E96" s="32" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="F96" s="32" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="G96" s="32"/>
       <c r="H96" s="32"/>
@@ -13053,7 +13052,7 @@
     <row r="97" customFormat="1" ht="15.5" spans="1:15">
       <c r="A97" s="26"/>
       <c r="B97" s="30" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C97" s="31" t="s">
         <v>30</v>
@@ -13062,10 +13061,10 @@
         <v>319</v>
       </c>
       <c r="E97" s="32" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="F97" s="32" t="s">
-        <v>945</v>
+        <v>931</v>
       </c>
       <c r="G97" s="32"/>
       <c r="H97" s="32"/>
@@ -13077,7 +13076,7 @@
       <c r="N97" s="71"/>
       <c r="O97" s="62"/>
     </row>
-    <row r="98" customFormat="1" ht="15.5" spans="1:15">
+    <row r="98" customFormat="1" ht="16.5" spans="1:15">
       <c r="A98" s="26"/>
       <c r="B98" s="30" t="s">
         <v>946</v>
@@ -13091,8 +13090,8 @@
       <c r="E98" s="32" t="s">
         <v>947</v>
       </c>
-      <c r="F98" s="32" t="s">
-        <v>933</v>
+      <c r="F98" s="80" t="s">
+        <v>926</v>
       </c>
       <c r="G98" s="32"/>
       <c r="H98" s="32"/>
@@ -13119,7 +13118,7 @@
         <v>949</v>
       </c>
       <c r="F99" s="80" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G99" s="32"/>
       <c r="H99" s="32"/>
@@ -13131,7 +13130,7 @@
       <c r="N99" s="71"/>
       <c r="O99" s="62"/>
     </row>
-    <row r="100" customFormat="1" ht="16.5" spans="1:15">
+    <row r="100" customFormat="1" ht="15.5" spans="1:15">
       <c r="A100" s="26"/>
       <c r="B100" s="30" t="s">
         <v>950</v>
@@ -13145,8 +13144,8 @@
       <c r="E100" s="32" t="s">
         <v>951</v>
       </c>
-      <c r="F100" s="80" t="s">
-        <v>928</v>
+      <c r="F100" s="32" t="s">
+        <v>952</v>
       </c>
       <c r="G100" s="32"/>
       <c r="H100" s="32"/>
@@ -13161,20 +13160,18 @@
     <row r="101" customFormat="1" ht="15.5" spans="1:15">
       <c r="A101" s="26"/>
       <c r="B101" s="30" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C101" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D101" s="32" t="s">
-        <v>319</v>
+        <v>253</v>
       </c>
       <c r="E101" s="32" t="s">
-        <v>953</v>
-      </c>
-      <c r="F101" s="32" t="s">
-        <v>933</v>
-      </c>
+        <v>954</v>
+      </c>
+      <c r="F101" s="32"/>
       <c r="G101" s="32"/>
       <c r="H101" s="32"/>
       <c r="I101" s="32"/>
@@ -13185,10 +13182,12 @@
       <c r="N101" s="71"/>
       <c r="O101" s="62"/>
     </row>
-    <row r="102" customFormat="1" ht="15.5" spans="1:15">
-      <c r="A102" s="26"/>
+    <row r="102" s="58" customFormat="1" ht="15.5" spans="1:15">
+      <c r="A102" s="26" t="s">
+        <v>955</v>
+      </c>
       <c r="B102" s="30" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="C102" s="31" t="s">
         <v>30</v>
@@ -13196,8 +13195,8 @@
       <c r="D102" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="E102" s="32" t="s">
-        <v>955</v>
+      <c r="E102" s="39" t="s">
+        <v>957</v>
       </c>
       <c r="F102" s="32"/>
       <c r="G102" s="32"/>
@@ -13210,22 +13209,12 @@
       <c r="N102" s="71"/>
       <c r="O102" s="62"/>
     </row>
-    <row r="103" s="58" customFormat="1" ht="15.5" spans="1:15">
-      <c r="A103" s="26" t="s">
-        <v>956</v>
-      </c>
-      <c r="B103" s="30" t="s">
-        <v>957</v>
-      </c>
-      <c r="C103" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D103" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="E103" s="39" t="s">
-        <v>958</v>
-      </c>
+    <row r="103" ht="23" customHeight="1" spans="1:15">
+      <c r="A103" s="26"/>
+      <c r="B103" s="30"/>
+      <c r="C103" s="31"/>
+      <c r="D103" s="32"/>
+      <c r="E103" s="32"/>
       <c r="F103" s="32"/>
       <c r="G103" s="32"/>
       <c r="H103" s="32"/>
@@ -14121,23 +14110,6 @@
       <c r="N155" s="71"/>
       <c r="O155" s="62"/>
     </row>
-    <row r="156" ht="23" customHeight="1" spans="1:15">
-      <c r="A156" s="26"/>
-      <c r="B156" s="30"/>
-      <c r="C156" s="31"/>
-      <c r="D156" s="32"/>
-      <c r="E156" s="32"/>
-      <c r="F156" s="32"/>
-      <c r="G156" s="32"/>
-      <c r="H156" s="32"/>
-      <c r="I156" s="32"/>
-      <c r="J156" s="73"/>
-      <c r="K156" s="62"/>
-      <c r="L156" s="71"/>
-      <c r="M156" s="72"/>
-      <c r="N156" s="71"/>
-      <c r="O156" s="62"/>
-    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -14179,345 +14151,345 @@
       <formula>LEFT(N11,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30">
+  <conditionalFormatting sqref="N29">
     <cfRule type="beginsWith" dxfId="0" priority="139" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N30,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N29,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="140" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N30,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N29,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="141" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N30,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N29,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N37">
+    <cfRule type="beginsWith" dxfId="0" priority="127" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N37,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="128" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N37,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="129" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N37,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38">
-    <cfRule type="beginsWith" dxfId="0" priority="127" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="211" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N38,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="128" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="212" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N38,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="129" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="213" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N38,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N39">
-    <cfRule type="beginsWith" dxfId="0" priority="211" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="121" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N39,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="212" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="122" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N39,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="213" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="123" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N39,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40">
-    <cfRule type="beginsWith" dxfId="0" priority="121" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="124" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N40,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="122" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="125" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N40,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="123" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="126" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N40,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41">
-    <cfRule type="beginsWith" dxfId="0" priority="124" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="259" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N41,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="125" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="260" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N41,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="126" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="261" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N41,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42">
-    <cfRule type="beginsWith" dxfId="0" priority="259" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="118" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N42,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="260" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="119" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N42,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="261" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="120" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N42,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43">
-    <cfRule type="beginsWith" dxfId="0" priority="118" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="205" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N43,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="119" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="206" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N43,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="120" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="207" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N43,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N44">
-    <cfRule type="beginsWith" dxfId="0" priority="205" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="115" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N44,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="206" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="116" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N44,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="207" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="117" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N44,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="beginsWith" dxfId="0" priority="115" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="199" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N45,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="116" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="200" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N45,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="117" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="201" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N45,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="beginsWith" dxfId="0" priority="199" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="193" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N46,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="200" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="194" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N46,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="201" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="195" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N46,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N47">
-    <cfRule type="beginsWith" dxfId="0" priority="193" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N47,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="194" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N47,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="195" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N47,LEN("PASS"))="PASS"</formula>
+  <conditionalFormatting sqref="N51">
+    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N51,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N51,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N51,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
-    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N52,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N52,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N52,LEN("WARN"))="WARN"</formula>
+  <conditionalFormatting sqref="N54">
+    <cfRule type="beginsWith" dxfId="0" priority="184" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N54,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="185" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N54,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="186" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N54,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55">
-    <cfRule type="beginsWith" dxfId="0" priority="184" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="91" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N55,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="185" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="92" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N55,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="186" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="93" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N55,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="beginsWith" dxfId="0" priority="91" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="109" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N56,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="92" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="110" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N56,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="93" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="111" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N56,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57">
-    <cfRule type="beginsWith" dxfId="0" priority="109" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="112" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N57,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="110" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="113" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N57,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="111" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="114" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N57,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N58">
-    <cfRule type="beginsWith" dxfId="0" priority="112" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="181" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N58,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="113" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="182" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N58,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="114" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="183" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N58,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N59">
-    <cfRule type="beginsWith" dxfId="0" priority="181" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="97" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N59,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="182" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="98" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N59,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="183" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="99" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N59,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N60">
-    <cfRule type="beginsWith" dxfId="0" priority="97" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N60,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="98" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N60,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="99" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N60,LEN("PASS"))="PASS"</formula>
+  <conditionalFormatting sqref="N67">
+    <cfRule type="beginsWith" dxfId="0" priority="94" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N67,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="95" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N67,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="96" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N67,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N68">
-    <cfRule type="beginsWith" dxfId="0" priority="94" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N68,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="95" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N68,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="96" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N68,LEN("PASS"))="PASS"</formula>
+  <conditionalFormatting sqref="N89">
+    <cfRule type="beginsWith" dxfId="0" priority="64" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N89,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="65" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N89,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="66" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N89,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N90">
-    <cfRule type="beginsWith" dxfId="0" priority="64" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="58" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N90,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="65" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="59" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N90,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="66" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="60" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N90,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N91">
-    <cfRule type="beginsWith" dxfId="0" priority="58" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="55" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N91,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="59" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="56" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N91,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="60" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="57" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N91,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N92">
-    <cfRule type="beginsWith" dxfId="0" priority="55" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N92,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="56" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N92,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="57" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N92,LEN("PASS"))="PASS"</formula>
+  <conditionalFormatting sqref="N94">
+    <cfRule type="beginsWith" dxfId="0" priority="52" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N94,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="53" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N94,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="54" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N94,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N95">
-    <cfRule type="beginsWith" dxfId="0" priority="52" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="49" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N95,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="53" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="50" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N95,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="54" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="51" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N95,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N96">
-    <cfRule type="beginsWith" dxfId="0" priority="49" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="46" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N96,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="50" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="47" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N96,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="51" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="48" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N96,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N97">
-    <cfRule type="beginsWith" dxfId="0" priority="46" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="40" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N97,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="47" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="41" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N97,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="48" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="42" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N97,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N98">
-    <cfRule type="beginsWith" dxfId="0" priority="40" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="37" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N98,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="41" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="38" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N98,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="42" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="39" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N98,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N99">
-    <cfRule type="beginsWith" dxfId="0" priority="37" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="34" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N99,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="38" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="35" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N99,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="39" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="36" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N99,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N100">
-    <cfRule type="beginsWith" dxfId="0" priority="34" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="31" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N100,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="35" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="32" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N100,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="36" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="33" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N100,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N101">
-    <cfRule type="beginsWith" dxfId="0" priority="31" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="22" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N101,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="32" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="23" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N101,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="33" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="24" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N101,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N102">
-    <cfRule type="beginsWith" dxfId="0" priority="22" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N102,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="23" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N102,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="24" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N102,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N103">
-    <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N103,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N103,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N103,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N4">
@@ -14586,7 +14558,7 @@
       <formula>LEFT(N17,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N20:N24">
+  <conditionalFormatting sqref="N20:N23">
     <cfRule type="beginsWith" dxfId="0" priority="244" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N20,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -14597,73 +14569,73 @@
       <formula>LEFT(N20,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N34:N36">
+  <conditionalFormatting sqref="N33:N35">
     <cfRule type="beginsWith" dxfId="0" priority="145" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N34,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N33,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="146" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N34,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N33,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="147" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N34,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N33,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N48:N49">
+  <conditionalFormatting sqref="N47:N48">
     <cfRule type="beginsWith" dxfId="0" priority="196" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N48,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N47,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="197" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N48,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N47,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="198" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N48,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N47,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50:N51">
+  <conditionalFormatting sqref="N49:N50">
     <cfRule type="beginsWith" dxfId="0" priority="190" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N50,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N49,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="191" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N50,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N49,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="192" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N50,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N49,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N76:N82">
+  <conditionalFormatting sqref="N75:N81">
     <cfRule type="beginsWith" dxfId="0" priority="88" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N76,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N75,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="89" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N76,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N75,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="90" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N76,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N75,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N83:N87">
+  <conditionalFormatting sqref="N82:N86">
     <cfRule type="beginsWith" dxfId="0" priority="19" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N83,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N82,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="20" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N83,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N82,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="21" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N83,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N82,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N104:N156">
+  <conditionalFormatting sqref="N103:N155">
     <cfRule type="beginsWith" dxfId="0" priority="290" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N104,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N103,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="291" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N104,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N103,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="292" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N104,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N103,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 N37 N53:N54">
+  <conditionalFormatting sqref="N1 N36 N52:N53">
     <cfRule type="beginsWith" dxfId="0" priority="293" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -14685,33 +14657,33 @@
       <formula>LEFT(N16,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N25:N29 N31:N33">
+  <conditionalFormatting sqref="N24:N28 N30:N32">
     <cfRule type="beginsWith" dxfId="0" priority="142" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N25,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N24,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="143" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N25,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N24,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="144" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N25,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N24,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N88:N89 N93:N94">
+  <conditionalFormatting sqref="N87:N88 N92:N93">
     <cfRule type="beginsWith" dxfId="0" priority="67" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N88,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N87,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="68" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N88,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N87,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="69" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N88,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N87,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C25 C26 C27 C30 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C22:C24 C28:C29 C31:C32 C53:C54 C104:C156">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C24 C25 C26 C29 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C22:C23 C27:C28 C30:C31 C52:C53 C103:C155">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D25 D26 D27 D30 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D22:D24 D28:D29 D31:D32 D33:D34 D53:D54 D104:D156">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D24 D25 D26 D29 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D22:D23 D27:D28 D30:D31 D32:D33 D52:D53 D103:D155">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
@@ -14725,10 +14697,10 @@
   <sheetPr/>
   <dimension ref="A1:O136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -14862,7 +14834,7 @@
     </row>
     <row r="5" ht="28" spans="1:15">
       <c r="A5" s="26" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>757</v>
@@ -15021,7 +14993,7 @@
     <row r="11" ht="23" customHeight="1" spans="1:15">
       <c r="A11" s="35"/>
       <c r="B11" s="30" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>30</v>
@@ -15030,7 +15002,7 @@
         <v>253</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="28"/>
@@ -15046,7 +15018,7 @@
     <row r="12" ht="23" customHeight="1" spans="1:15">
       <c r="A12"/>
       <c r="B12" s="30" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C12" s="36" t="s">
         <v>30</v>
@@ -15055,7 +15027,7 @@
         <v>576</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>763</v>
@@ -15073,7 +15045,7 @@
     <row r="13" ht="23" customHeight="1" spans="1:15">
       <c r="A13" s="26"/>
       <c r="B13" s="30" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>30</v>
@@ -15082,7 +15054,7 @@
         <v>576</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="F13" s="32" t="s">
         <v>763</v>
@@ -15112,7 +15084,7 @@
         <v>774</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
@@ -15319,7 +15291,7 @@
         <v>576</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F22" s="33">
         <v>2000</v>
@@ -15337,7 +15309,7 @@
     <row r="23" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="20"/>
       <c r="B23" s="21" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>5</v>
@@ -15346,10 +15318,10 @@
         <v>471</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G23" s="41"/>
       <c r="K23" s="62"/>
@@ -15361,7 +15333,7 @@
     <row r="24" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="26"/>
       <c r="B24" s="21" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C24" s="31" t="s">
         <v>30</v>
@@ -15370,10 +15342,10 @@
         <v>706</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G24" s="32"/>
       <c r="K24" s="62"/>
@@ -15385,7 +15357,7 @@
     <row r="25" ht="23" customHeight="1" spans="1:15">
       <c r="A25" s="26"/>
       <c r="B25" s="21" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>30</v>
@@ -15394,10 +15366,10 @@
         <v>706</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="G25" s="32"/>
       <c r="K25" s="62"/>
@@ -15409,7 +15381,7 @@
     <row r="26" ht="23" customHeight="1" spans="1:15">
       <c r="A26" s="26"/>
       <c r="B26" s="21" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C26" s="31" t="s">
         <v>30</v>
@@ -15418,10 +15390,10 @@
         <v>706</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G26" s="32"/>
       <c r="K26" s="62"/>
@@ -15433,7 +15405,7 @@
     <row r="27" ht="23" customHeight="1" spans="1:15">
       <c r="A27" s="26"/>
       <c r="B27" s="21" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C27" s="31" t="s">
         <v>30</v>
@@ -15442,10 +15414,10 @@
         <v>706</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="G27" s="32"/>
       <c r="K27" s="62"/>
@@ -15457,7 +15429,7 @@
     <row r="28" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="26"/>
       <c r="B28" s="21" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C28" s="31" t="s">
         <v>30</v>
@@ -15466,10 +15438,10 @@
         <v>706</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="G28" s="32"/>
       <c r="K28" s="62"/>
@@ -15481,7 +15453,7 @@
     <row r="29" ht="23" customHeight="1" spans="1:15">
       <c r="A29" s="26"/>
       <c r="B29" s="21" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>30</v>
@@ -15490,10 +15462,10 @@
         <v>706</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="G29" s="32"/>
       <c r="K29" s="62"/>
@@ -15505,7 +15477,7 @@
     <row r="30" ht="23" customHeight="1" spans="1:15">
       <c r="A30" s="26"/>
       <c r="B30" s="21" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C30" s="31" t="s">
         <v>30</v>
@@ -15514,7 +15486,7 @@
         <v>576</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F30" s="33">
         <v>2000</v>
@@ -15529,7 +15501,7 @@
     <row r="31" ht="23" customHeight="1" spans="1:15">
       <c r="A31" s="26"/>
       <c r="B31" s="30" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C31" s="31" t="s">
         <v>30</v>
@@ -15538,7 +15510,7 @@
         <v>576</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F31" s="33">
         <v>2000</v>
@@ -15581,7 +15553,7 @@
     <row r="33" ht="23" customHeight="1" spans="1:15">
       <c r="A33" s="26"/>
       <c r="B33" s="30" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C33" s="31" t="s">
         <v>30</v>
@@ -15590,7 +15562,7 @@
         <v>253</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="32"/>
@@ -15606,7 +15578,7 @@
     <row r="34" ht="23" customHeight="1" spans="1:15">
       <c r="A34" s="26"/>
       <c r="B34" s="30" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="C34" s="31" t="s">
         <v>30</v>
@@ -15615,10 +15587,10 @@
         <v>576</v>
       </c>
       <c r="E34" s="32" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
@@ -15658,7 +15630,7 @@
     <row r="36" ht="23" customHeight="1" spans="1:15">
       <c r="A36" s="26"/>
       <c r="B36" s="30" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C36" s="31" t="s">
         <v>30</v>
@@ -15667,7 +15639,7 @@
         <v>576</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F36" s="33">
         <v>2000</v>
@@ -15685,7 +15657,7 @@
     <row r="37" ht="23" customHeight="1" spans="1:15">
       <c r="A37" s="26"/>
       <c r="B37" s="30" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>30</v>
@@ -15694,7 +15666,7 @@
         <v>253</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="F37" s="33"/>
       <c r="G37" s="32"/>
@@ -15735,7 +15707,7 @@
     <row r="39" ht="23" customHeight="1" spans="1:15">
       <c r="A39" s="1"/>
       <c r="B39" s="21" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>30</v>
@@ -15744,10 +15716,10 @@
         <v>493</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
@@ -15762,7 +15734,7 @@
     <row r="40" ht="23" customHeight="1" spans="1:15">
       <c r="A40" s="1"/>
       <c r="B40" s="21" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>5</v>
@@ -15771,7 +15743,7 @@
         <v>536</v>
       </c>
       <c r="E40" s="32" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
@@ -15787,7 +15759,7 @@
     <row r="41" ht="23" customHeight="1" spans="1:15">
       <c r="A41" s="1"/>
       <c r="B41" s="21" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>30</v>
@@ -15796,7 +15768,7 @@
         <v>576</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="F41" s="33">
         <v>2000</v>
@@ -15813,7 +15785,7 @@
     </row>
     <row r="42" ht="28" spans="1:15">
       <c r="A42" s="26" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>757</v>
@@ -15843,7 +15815,7 @@
     <row r="43" ht="23" customHeight="1" spans="1:15">
       <c r="A43" s="42"/>
       <c r="B43" s="21" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>30</v>
@@ -15852,7 +15824,7 @@
         <v>576</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="F43" s="29">
         <v>2000</v>
@@ -15904,7 +15876,7 @@
         <v>576</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="F45" s="33">
         <v>2000</v>
@@ -15947,7 +15919,7 @@
     <row r="47" ht="23" customHeight="1" spans="1:15">
       <c r="A47"/>
       <c r="B47" s="30" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C47" s="36" t="s">
         <v>30</v>
@@ -15956,7 +15928,7 @@
         <v>576</v>
       </c>
       <c r="E47" s="37" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="F47" s="32" t="s">
         <v>763</v>
@@ -15974,7 +15946,7 @@
     <row r="48" ht="23" customHeight="1" spans="1:15">
       <c r="A48" s="43"/>
       <c r="B48" s="44" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C48" s="45" t="s">
         <v>30</v>
@@ -15983,10 +15955,10 @@
         <v>692</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="G48" s="47"/>
       <c r="H48" s="47"/>
@@ -16001,19 +15973,19 @@
     <row r="49" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A49" s="48"/>
       <c r="B49" s="49" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="C49" s="50" t="s">
         <v>30</v>
       </c>
       <c r="D49" s="51" t="s">
-        <v>253</v>
+        <v>530</v>
       </c>
       <c r="E49" s="52" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="F49" s="53" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G49" s="54"/>
       <c r="H49" s="54"/>
@@ -16028,7 +16000,7 @@
     <row r="50" ht="23" customHeight="1" spans="1:15">
       <c r="A50" s="26"/>
       <c r="B50" s="30" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="C50" s="31" t="s">
         <v>30</v>
@@ -16037,10 +16009,10 @@
         <v>706</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="G50" s="32"/>
       <c r="H50" s="32"/>
@@ -16055,7 +16027,7 @@
     <row r="51" ht="23" customHeight="1" spans="1:15">
       <c r="A51" s="26"/>
       <c r="B51" s="30" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C51" s="31" t="s">
         <v>30</v>
@@ -16064,7 +16036,7 @@
         <v>363</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="F51" s="32"/>
       <c r="G51" s="32"/>
@@ -16080,7 +16052,7 @@
     <row r="52" ht="23" customHeight="1" spans="1:15">
       <c r="A52" s="26"/>
       <c r="B52" s="30" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>30</v>
@@ -16089,7 +16061,7 @@
         <v>576</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F52" s="33">
         <v>2000</v>
@@ -16132,7 +16104,7 @@
     <row r="54" ht="23" customHeight="1" spans="1:15">
       <c r="A54" s="1"/>
       <c r="B54" s="21" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C54" s="27" t="s">
         <v>30</v>
@@ -16141,10 +16113,10 @@
         <v>493</v>
       </c>
       <c r="E54" s="55" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
@@ -16159,7 +16131,7 @@
     <row r="55" ht="23" customHeight="1" spans="1:15">
       <c r="A55" s="26"/>
       <c r="B55" s="56" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C55" s="27" t="s">
         <v>30</v>
@@ -16168,7 +16140,7 @@
         <v>253</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="F55" s="55"/>
       <c r="G55" s="57"/>
@@ -16184,7 +16156,7 @@
     <row r="56" ht="23" customHeight="1" spans="1:15">
       <c r="A56" s="1"/>
       <c r="B56" s="21" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C56" s="27" t="s">
         <v>30</v>
@@ -16193,7 +16165,7 @@
         <v>576</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="F56" s="33">
         <v>2000</v>
@@ -16210,10 +16182,10 @@
     </row>
     <row r="57" ht="23" customHeight="1" spans="1:15">
       <c r="A57" s="20" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C57" s="31" t="s">
         <v>30</v>
@@ -16222,7 +16194,7 @@
         <v>363</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="F57" s="58"/>
       <c r="G57" s="33"/>
@@ -16238,7 +16210,7 @@
     <row r="58" ht="23" customHeight="1" spans="1:15">
       <c r="A58"/>
       <c r="B58" s="21" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C58" s="27" t="s">
         <v>30</v>
@@ -16247,10 +16219,10 @@
         <v>576</v>
       </c>
       <c r="E58" s="32" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="F58" s="37" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="G58" s="32"/>
       <c r="H58" s="28"/>
@@ -16265,7 +16237,7 @@
     <row r="59" ht="23" customHeight="1" spans="1:15">
       <c r="A59" s="20"/>
       <c r="B59" s="21" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C59" s="27" t="s">
         <v>30</v>
@@ -16274,7 +16246,7 @@
         <v>363</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F59" s="28"/>
       <c r="G59" s="32"/>
@@ -16290,7 +16262,7 @@
     <row r="60" ht="23" customHeight="1" spans="1:15">
       <c r="A60" s="20"/>
       <c r="B60" s="59" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="C60" s="36" t="s">
         <v>30</v>
@@ -16299,7 +16271,7 @@
         <v>363</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="F60" s="60"/>
       <c r="G60" s="32"/>
@@ -16315,7 +16287,7 @@
     <row r="61" ht="23" customHeight="1" spans="1:15">
       <c r="A61" s="20"/>
       <c r="B61" s="21" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C61" s="27" t="s">
         <v>30</v>
@@ -16324,7 +16296,7 @@
         <v>714</v>
       </c>
       <c r="E61" s="28" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="F61" s="40"/>
       <c r="G61" s="32"/>
@@ -16340,7 +16312,7 @@
     <row r="62" ht="23" customHeight="1" spans="1:15">
       <c r="A62" s="20"/>
       <c r="B62" s="59" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C62" s="36" t="s">
         <v>30</v>
@@ -16349,7 +16321,7 @@
         <v>363</v>
       </c>
       <c r="E62" s="28" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="F62" s="60"/>
       <c r="G62" s="32"/>
@@ -16365,7 +16337,7 @@
     <row r="63" ht="23" customHeight="1" spans="1:15">
       <c r="A63" s="20"/>
       <c r="B63" s="21" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>30</v>
@@ -16374,7 +16346,7 @@
         <v>714</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="F63" s="60"/>
       <c r="G63" s="32"/>
@@ -16390,7 +16362,7 @@
     <row r="64" ht="23" customHeight="1" spans="1:15">
       <c r="A64" s="20"/>
       <c r="B64" s="59" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="C64" s="36" t="s">
         <v>30</v>
@@ -16399,7 +16371,7 @@
         <v>363</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F64" s="60"/>
       <c r="G64" s="32"/>
@@ -16415,7 +16387,7 @@
     <row r="65" ht="23" customHeight="1" spans="1:15">
       <c r="A65" s="26"/>
       <c r="B65" s="30" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="C65" s="36" t="s">
         <v>5</v>
@@ -16424,10 +16396,10 @@
         <v>471</v>
       </c>
       <c r="E65" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="F65" s="55" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="G65" s="32"/>
       <c r="H65" s="32"/>
@@ -16442,7 +16414,7 @@
     <row r="66" ht="23" customHeight="1" spans="1:15">
       <c r="A66" s="20"/>
       <c r="B66" s="59" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C66" s="36" t="s">
         <v>30</v>
@@ -16451,10 +16423,10 @@
         <v>706</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="F66" s="60" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="G66" s="32"/>
       <c r="H66" s="28"/>
@@ -16469,7 +16441,7 @@
     <row r="67" ht="23" customHeight="1" spans="1:15">
       <c r="A67" s="20"/>
       <c r="B67" s="59" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C67" s="36" t="s">
         <v>30</v>
@@ -16478,10 +16450,10 @@
         <v>706</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="F67" s="60" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="G67" s="32"/>
       <c r="H67" s="28"/>
@@ -16496,7 +16468,7 @@
     <row r="68" ht="23" customHeight="1" spans="1:15">
       <c r="A68" s="20"/>
       <c r="B68" s="21" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="C68" s="27" t="s">
         <v>5</v>
@@ -16505,16 +16477,16 @@
         <v>486</v>
       </c>
       <c r="E68" s="70" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F68" s="79" t="s">
         <v>752</v>
       </c>
       <c r="G68" s="55" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="H68" s="58" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="I68" s="58"/>
       <c r="J68" s="58"/>
@@ -16527,7 +16499,7 @@
     <row r="69" ht="23" customHeight="1" spans="1:15">
       <c r="A69" s="20"/>
       <c r="B69" s="21" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C69" s="27" t="s">
         <v>30</v>
@@ -16536,7 +16508,7 @@
         <v>363</v>
       </c>
       <c r="E69" s="70" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="F69" s="33"/>
       <c r="G69" s="32"/>
@@ -16552,7 +16524,7 @@
     <row r="70" ht="23" customHeight="1" spans="1:15">
       <c r="A70" s="20"/>
       <c r="B70" s="21" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C70" s="27" t="s">
         <v>30</v>
@@ -16561,7 +16533,7 @@
         <v>714</v>
       </c>
       <c r="E70" s="28" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="F70" s="60"/>
       <c r="G70" s="32"/>
@@ -16577,7 +16549,7 @@
     <row r="71" ht="23" customHeight="1" spans="1:15">
       <c r="A71" s="26"/>
       <c r="B71" s="21" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="C71" s="27" t="s">
         <v>30</v>
@@ -16586,13 +16558,13 @@
         <v>650</v>
       </c>
       <c r="E71" t="s">
+        <v>878</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>879</v>
+      </c>
+      <c r="G71" s="55" t="s">
         <v>880</v>
-      </c>
-      <c r="F71" s="32" t="s">
-        <v>881</v>
-      </c>
-      <c r="G71" s="55" t="s">
-        <v>882</v>
       </c>
       <c r="H71" s="58"/>
       <c r="I71" s="32"/>
@@ -16606,7 +16578,7 @@
     <row r="72" ht="23" customHeight="1" spans="1:15">
       <c r="A72" s="20"/>
       <c r="B72" s="21" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="C72" s="27" t="s">
         <v>5</v>
@@ -16615,10 +16587,10 @@
         <v>49</v>
       </c>
       <c r="E72" s="70" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="F72" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="G72" s="32"/>
       <c r="H72" s="58"/>
@@ -16632,10 +16604,10 @@
     </row>
     <row r="73" ht="42" spans="1:15">
       <c r="A73" s="26" t="s">
+        <v>973</v>
+      </c>
+      <c r="B73" s="30" t="s">
         <v>974</v>
-      </c>
-      <c r="B73" s="30" t="s">
-        <v>975</v>
       </c>
       <c r="C73" s="31" t="s">
         <v>30</v>
@@ -16644,7 +16616,7 @@
         <v>253</v>
       </c>
       <c r="E73" s="32" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="F73" s="32"/>
       <c r="G73" s="32"/>
@@ -16660,7 +16632,7 @@
     <row r="74" ht="23" customHeight="1" spans="1:15">
       <c r="A74" s="26"/>
       <c r="B74" s="30" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C74" s="31" t="s">
         <v>30</v>
@@ -16669,10 +16641,10 @@
         <v>319</v>
       </c>
       <c r="E74" s="32" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="F74" s="32" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="G74" s="32"/>
       <c r="H74" s="32"/>
@@ -16687,7 +16659,7 @@
     <row r="75" ht="23" customHeight="1" spans="1:15">
       <c r="A75" s="26"/>
       <c r="B75" s="30" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C75" s="31" t="s">
         <v>30</v>
@@ -16696,7 +16668,7 @@
         <v>319</v>
       </c>
       <c r="E75" s="32" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>782</v>
@@ -16714,7 +16686,7 @@
     <row r="76" ht="23" customHeight="1" spans="1:15">
       <c r="A76" s="26"/>
       <c r="B76" s="30" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="C76" s="31" t="s">
         <v>30</v>
@@ -16723,10 +16695,10 @@
         <v>319</v>
       </c>
       <c r="E76" s="32" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="G76" s="32"/>
       <c r="H76" s="32"/>
@@ -16741,7 +16713,7 @@
     <row r="77" ht="23" customHeight="1" spans="1:15">
       <c r="A77" s="26"/>
       <c r="B77" s="30" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C77" s="31" t="s">
         <v>30</v>
@@ -16750,10 +16722,10 @@
         <v>319</v>
       </c>
       <c r="E77" s="32" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="G77" s="32"/>
       <c r="H77" s="32"/>
@@ -16768,7 +16740,7 @@
     <row r="78" ht="23" customHeight="1" spans="1:15">
       <c r="A78" s="26"/>
       <c r="B78" s="30" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C78" s="31" t="s">
         <v>30</v>
@@ -16777,10 +16749,10 @@
         <v>319</v>
       </c>
       <c r="E78" s="32" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="G78" s="32"/>
       <c r="H78" s="32"/>
@@ -16795,7 +16767,7 @@
     <row r="79" ht="23" customHeight="1" spans="1:15">
       <c r="A79" s="26"/>
       <c r="B79" s="30" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="C79" s="31" t="s">
         <v>30</v>
@@ -16804,10 +16776,10 @@
         <v>319</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="F79" s="29" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="G79" s="32"/>
       <c r="H79" s="32"/>
@@ -16822,7 +16794,7 @@
     <row r="80" ht="23" customHeight="1" spans="1:15">
       <c r="A80" s="26"/>
       <c r="B80" s="30" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C80" s="31" t="s">
         <v>30</v>
@@ -16831,10 +16803,10 @@
         <v>319</v>
       </c>
       <c r="E80" s="32" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G80" s="32"/>
       <c r="H80" s="32"/>
@@ -16849,7 +16821,7 @@
     <row r="81" ht="23" customHeight="1" spans="1:15">
       <c r="A81" s="26"/>
       <c r="B81" s="30" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C81" s="31" t="s">
         <v>5</v>
@@ -16858,10 +16830,10 @@
         <v>471</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="G81" s="32"/>
       <c r="H81" s="32"/>
@@ -16876,7 +16848,7 @@
     <row r="82" ht="23" customHeight="1" spans="1:15">
       <c r="A82" s="26"/>
       <c r="B82" s="30" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C82" s="31" t="s">
         <v>30</v>
@@ -16885,10 +16857,10 @@
         <v>319</v>
       </c>
       <c r="E82" s="32" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="G82" s="32"/>
       <c r="H82" s="32"/>
@@ -16903,7 +16875,7 @@
     <row r="83" ht="23" customHeight="1" spans="1:15">
       <c r="A83" s="26"/>
       <c r="B83" s="30" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C83" s="31" t="s">
         <v>30</v>
@@ -16912,10 +16884,10 @@
         <v>319</v>
       </c>
       <c r="E83" s="32" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="G83" s="32"/>
       <c r="H83" s="32"/>
@@ -16930,7 +16902,7 @@
     <row r="84" ht="23" customHeight="1" spans="1:15">
       <c r="A84" s="26"/>
       <c r="B84" s="30" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C84" s="31" t="s">
         <v>30</v>
@@ -16939,10 +16911,10 @@
         <v>319</v>
       </c>
       <c r="E84" s="32" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="F84" s="29" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="G84" s="32"/>
       <c r="H84" s="32"/>
@@ -16957,7 +16929,7 @@
     <row r="85" ht="23" customHeight="1" spans="1:15">
       <c r="A85" s="26"/>
       <c r="B85" s="30" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C85" s="31" t="s">
         <v>30</v>
@@ -16966,10 +16938,10 @@
         <v>319</v>
       </c>
       <c r="E85" s="32" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F85" s="32" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G85" s="32"/>
       <c r="H85" s="32"/>
@@ -16984,7 +16956,7 @@
     <row r="86" ht="23" customHeight="1" spans="1:15">
       <c r="A86" s="26"/>
       <c r="B86" s="30" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C86" s="31" t="s">
         <v>30</v>
@@ -16993,10 +16965,10 @@
         <v>535</v>
       </c>
       <c r="E86" s="32" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="F86" s="32" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="G86" s="32"/>
       <c r="H86" s="32"/>
@@ -17011,7 +16983,7 @@
     <row r="87" ht="23" customHeight="1" spans="1:15">
       <c r="A87" s="26"/>
       <c r="B87" s="30" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C87" s="31" t="s">
         <v>30</v>
@@ -17020,10 +16992,10 @@
         <v>319</v>
       </c>
       <c r="E87" s="32" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="F87" s="32" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="G87" s="32"/>
       <c r="H87" s="32"/>
@@ -17038,7 +17010,7 @@
     <row r="88" ht="23" customHeight="1" spans="1:15">
       <c r="A88" s="26"/>
       <c r="B88" s="30" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C88" s="31" t="s">
         <v>30</v>
@@ -17047,10 +17019,10 @@
         <v>319</v>
       </c>
       <c r="E88" s="32" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="F88" s="80" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G88" s="32"/>
       <c r="H88" s="32"/>
@@ -17065,7 +17037,7 @@
     <row r="89" ht="23" customHeight="1" spans="1:15">
       <c r="A89" s="26"/>
       <c r="B89" s="30" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C89" s="31" t="s">
         <v>30</v>
@@ -17074,10 +17046,10 @@
         <v>319</v>
       </c>
       <c r="E89" s="32" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="F89" s="80" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G89" s="32"/>
       <c r="H89" s="32"/>
@@ -17092,7 +17064,7 @@
     <row r="90" ht="23" customHeight="1" spans="1:15">
       <c r="A90" s="26"/>
       <c r="B90" s="30" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C90" s="31" t="s">
         <v>30</v>
@@ -17101,10 +17073,10 @@
         <v>319</v>
       </c>
       <c r="E90" s="32" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="F90" s="32" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G90" s="32"/>
       <c r="H90" s="32"/>
@@ -17119,7 +17091,7 @@
     <row r="91" ht="23" customHeight="1" spans="1:15">
       <c r="A91" s="26"/>
       <c r="B91" s="30" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C91" s="31" t="s">
         <v>30</v>
@@ -17128,10 +17100,10 @@
         <v>319</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="F91" s="32" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="G91" s="32"/>
       <c r="H91" s="32"/>
@@ -17146,7 +17118,7 @@
     <row r="92" ht="23" customHeight="1" spans="1:15">
       <c r="A92" s="26"/>
       <c r="B92" s="30" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C92" s="31" t="s">
         <v>30</v>
@@ -17155,10 +17127,10 @@
         <v>319</v>
       </c>
       <c r="E92" s="32" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="F92" s="32" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="G92" s="32"/>
       <c r="H92" s="32"/>
@@ -17173,7 +17145,7 @@
     <row r="93" ht="23" customHeight="1" spans="1:15">
       <c r="A93" s="26"/>
       <c r="B93" s="30" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C93" s="31" t="s">
         <v>30</v>
@@ -17182,10 +17154,10 @@
         <v>319</v>
       </c>
       <c r="E93" s="32" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="F93" s="32" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="G93" s="32"/>
       <c r="H93" s="32"/>
@@ -17200,7 +17172,7 @@
     <row r="94" ht="23" customHeight="1" spans="1:15">
       <c r="A94" s="26"/>
       <c r="B94" s="30" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C94" s="31" t="s">
         <v>30</v>
@@ -17209,10 +17181,10 @@
         <v>319</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="F94" s="32" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="G94" s="32"/>
       <c r="H94" s="32"/>
@@ -17227,7 +17199,7 @@
     <row r="95" ht="23" customHeight="1" spans="1:15">
       <c r="A95" s="26"/>
       <c r="B95" s="30" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C95" s="31" t="s">
         <v>30</v>
@@ -17236,10 +17208,10 @@
         <v>319</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F95" s="32" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G95" s="32"/>
       <c r="H95" s="32"/>
@@ -17254,7 +17226,7 @@
     <row r="96" ht="23" customHeight="1" spans="1:15">
       <c r="A96" s="26"/>
       <c r="B96" s="30" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C96" s="31" t="s">
         <v>30</v>
@@ -17263,10 +17235,10 @@
         <v>319</v>
       </c>
       <c r="E96" s="32" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="F96" s="80" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G96" s="32"/>
       <c r="H96" s="32"/>
@@ -17281,7 +17253,7 @@
     <row r="97" ht="23" customHeight="1" spans="1:15">
       <c r="A97" s="26"/>
       <c r="B97" s="30" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C97" s="31" t="s">
         <v>30</v>
@@ -17290,10 +17262,10 @@
         <v>319</v>
       </c>
       <c r="E97" s="32" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="F97" s="80" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G97" s="32"/>
       <c r="H97" s="32"/>
@@ -17308,7 +17280,7 @@
     <row r="98" ht="23" customHeight="1" spans="1:15">
       <c r="A98" s="26"/>
       <c r="B98" s="30" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C98" s="31" t="s">
         <v>30</v>
@@ -17317,10 +17289,10 @@
         <v>319</v>
       </c>
       <c r="E98" s="32" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="F98" s="32" t="s">
-        <v>933</v>
+        <v>952</v>
       </c>
       <c r="G98" s="32"/>
       <c r="H98" s="32"/>
@@ -17335,7 +17307,7 @@
     <row r="99" ht="23" customHeight="1" spans="1:15">
       <c r="A99" s="26"/>
       <c r="B99" s="30" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C99" s="31" t="s">
         <v>30</v>
@@ -17344,7 +17316,7 @@
         <v>253</v>
       </c>
       <c r="E99" s="32" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F99" s="32"/>
       <c r="G99" s="32"/>
@@ -17359,10 +17331,10 @@
     </row>
     <row r="100" ht="23" customHeight="1" spans="1:15">
       <c r="A100" s="26" t="s">
+        <v>955</v>
+      </c>
+      <c r="B100" s="30" t="s">
         <v>956</v>
-      </c>
-      <c r="B100" s="30" t="s">
-        <v>957</v>
       </c>
       <c r="C100" s="31" t="s">
         <v>30</v>
@@ -17371,7 +17343,7 @@
         <v>253</v>
       </c>
       <c r="E100" s="39" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F100" s="32"/>
       <c r="G100" s="32"/>

</xml_diff>